<commit_message>
correct scenario in data page
</commit_message>
<xml_diff>
--- a/meta/dimension.xlsx
+++ b/meta/dimension.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yildiz\Dropbox\PC\Documents\GitHub\wcde-shiny-2023\meta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guy\Dropbox\WCDE for Guy\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49281192-DD38-49C6-9975-54E777728B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7F3CD5-6B3C-4DB4-AD3C-7786DFCBEA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2205" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dimension" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="96">
   <si>
     <t>dim</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>Population Component of Conventional Development (SSP5): This scenario is similar to SSP1 for the fertility, mortality and education assumptions except that it combines them with high migration scenario in a context of widespread globalization.</t>
+  </si>
+  <si>
+    <t>wcde_code</t>
   </si>
 </sst>
 </file>
@@ -789,10 +792,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1138,19 +1140,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:XFD74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="42.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1164,13 +1166,16 @@
         <v>63</v>
       </c>
       <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1183,14 +1188,17 @@
       <c r="D2" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>67</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1203,14 +1211,17 @@
       <c r="D3" t="s">
         <v>65</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>71</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1223,14 +1234,17 @@
       <c r="D4" t="s">
         <v>66</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
         <v>72</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1243,14 +1257,17 @@
       <c r="D5" t="s">
         <v>88</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
         <v>73</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1263,14 +1280,17 @@
       <c r="D6" t="s">
         <v>87</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
         <v>74</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1283,11 +1303,14 @@
       <c r="D7" t="s">
         <v>90</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1300,11 +1323,14 @@
       <c r="D8" t="s">
         <v>92</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1314,11 +1340,11 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>-9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1328,11 +1354,11 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1342,11 +1368,11 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1356,11 +1382,11 @@
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1370,11 +1396,11 @@
       <c r="C13">
         <v>4</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1384,11 +1410,11 @@
       <c r="C14">
         <v>5</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1398,11 +1424,11 @@
       <c r="C15">
         <v>6</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1412,11 +1438,11 @@
       <c r="C16">
         <v>7</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1426,11 +1452,11 @@
       <c r="C17">
         <v>8</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1440,11 +1466,11 @@
       <c r="C18">
         <v>9</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1454,11 +1480,11 @@
       <c r="C19">
         <v>10</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1468,11 +1494,11 @@
       <c r="C20">
         <v>11</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1482,11 +1508,11 @@
       <c r="C21">
         <v>12</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1496,11 +1522,11 @@
       <c r="C22">
         <v>13</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1510,11 +1536,11 @@
       <c r="C23">
         <v>14</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1524,11 +1550,11 @@
       <c r="C24">
         <v>15</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1538,11 +1564,11 @@
       <c r="C25">
         <v>16</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1552,11 +1578,11 @@
       <c r="C26">
         <v>17</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1566,11 +1592,11 @@
       <c r="C27">
         <v>18</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1580,11 +1606,11 @@
       <c r="C28">
         <v>19</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1594,11 +1620,11 @@
       <c r="C29">
         <v>20</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1608,11 +1634,11 @@
       <c r="C30">
         <v>21</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1622,11 +1648,11 @@
       <c r="C31">
         <v>0</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>-9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1636,11 +1662,11 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1650,11 +1676,11 @@
       <c r="C33">
         <v>2</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1664,11 +1690,11 @@
       <c r="C34">
         <v>3</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>1500</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -1678,11 +1704,11 @@
       <c r="C35">
         <v>4</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>2500</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1692,11 +1718,11 @@
       <c r="C36">
         <v>5</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>2039</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -1706,11 +1732,11 @@
       <c r="C37">
         <v>6</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>4064</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -1720,11 +1746,11 @@
       <c r="C38">
         <v>7</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>6000</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -1734,11 +1760,11 @@
       <c r="C39">
         <v>8</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>6500</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1748,11 +1774,11 @@
       <c r="C40">
         <v>9</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>8000</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1762,11 +1788,11 @@
       <c r="C41">
         <v>10</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>2064</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -1776,11 +1802,11 @@
       <c r="C42">
         <v>0</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>-5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -1790,11 +1816,11 @@
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -1804,11 +1830,11 @@
       <c r="C44">
         <v>2</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1818,11 +1844,11 @@
       <c r="C45">
         <v>3</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>37</v>
       </c>
@@ -1832,11 +1858,11 @@
       <c r="C46">
         <v>4</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1846,11 +1872,11 @@
       <c r="C47">
         <v>5</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -1860,11 +1886,11 @@
       <c r="C48">
         <v>6</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -1874,11 +1900,11 @@
       <c r="C49">
         <v>7</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -1888,11 +1914,11 @@
       <c r="C50">
         <v>8</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -1902,11 +1928,11 @@
       <c r="C51">
         <v>9</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -1916,11 +1942,11 @@
       <c r="C52">
         <v>10</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -1930,11 +1956,11 @@
       <c r="C53">
         <v>11</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -1944,11 +1970,11 @@
       <c r="C54">
         <v>12</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -1958,11 +1984,11 @@
       <c r="C55">
         <v>13</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -1972,11 +1998,11 @@
       <c r="C56">
         <v>14</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -1986,11 +2012,11 @@
       <c r="C57">
         <v>15</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>37</v>
       </c>
@@ -2000,11 +2026,11 @@
       <c r="C58">
         <v>16</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -2014,11 +2040,11 @@
       <c r="C59">
         <v>17</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -2028,11 +2054,11 @@
       <c r="C60">
         <v>18</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>37</v>
       </c>
@@ -2042,11 +2068,11 @@
       <c r="C61">
         <v>19</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -2056,11 +2082,11 @@
       <c r="C62">
         <v>20</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -2070,11 +2096,11 @@
       <c r="C63">
         <v>21</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>38</v>
       </c>
@@ -2084,11 +2110,11 @@
       <c r="C64">
         <v>0</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>-9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -2098,11 +2124,11 @@
       <c r="C65">
         <v>1</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -2112,11 +2138,11 @@
       <c r="C66">
         <v>2</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>41</v>
       </c>
@@ -2126,14 +2152,14 @@
       <c r="C67">
         <v>0</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>42</v>
       </c>
-      <c r="F67">
+      <c r="G67">
         <v>-9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>41</v>
       </c>
@@ -2143,11 +2169,11 @@
       <c r="C68">
         <v>1</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>41</v>
       </c>
@@ -2157,14 +2183,14 @@
       <c r="C69">
         <v>2</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>45</v>
       </c>
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>41</v>
       </c>
@@ -2174,14 +2200,14 @@
       <c r="C70">
         <v>3</v>
       </c>
-      <c r="E70" t="s">
+      <c r="F70" t="s">
         <v>47</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>41</v>
       </c>
@@ -2191,14 +2217,14 @@
       <c r="C71">
         <v>4</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>49</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>41</v>
       </c>
@@ -2208,14 +2234,14 @@
       <c r="C72">
         <v>5</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>51</v>
       </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>41</v>
       </c>
@@ -2225,27 +2251,27 @@
       <c r="C73">
         <v>6</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
         <v>84</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="2" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>41</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" t="s">
         <v>53</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74">
         <v>7</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="F74" t="s">
         <v>70</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="G74" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
try again for wcde_code in dimen
</commit_message>
<xml_diff>
--- a/meta/dimension.xlsx
+++ b/meta/dimension.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guy\Dropbox\WCDE for Guy\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7F3CD5-6B3C-4DB4-AD3C-7786DFCBEA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7A8862-0A3B-42CE-9C69-C9667EEBDD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -295,9 +295,6 @@
     <t>SSP4</t>
   </si>
   <si>
-    <t>Conventional development (SSP5)</t>
-  </si>
-  <si>
     <t>SSP5</t>
   </si>
   <si>
@@ -308,6 +305,9 @@
   </si>
   <si>
     <t>wcde_code</t>
+  </si>
+  <si>
+    <t>Conventional Development (SSP5)</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1143,7 @@
   <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1166,7 +1166,7 @@
         <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1307,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1315,19 +1315,19 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C8">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update to meta files and tweaks
</commit_message>
<xml_diff>
--- a/meta/dimension.xlsx
+++ b/meta/dimension.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guy\Dropbox\WCDE for Guy\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7A8862-0A3B-42CE-9C69-C9667EEBDD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B031E3B3-0D4C-42D8-B996-A1C3C653E05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -241,12 +241,6 @@
     <t>Population Component of Stalled Development (SSP3): This scenario portrays a world separated into regions characterised by extreme poverty, pockets of moderate wealth, and many countries struggling to maintain living standards for rapidly growing populations.  This is associated with low education, high mortality and high fertility. Due to the emphasis on security and barriers to international exchange, migration is assumed to be low for all countries.</t>
   </si>
   <si>
-    <t>Population Component of Medium (SSP2): This is the middle of the road scenario with Zero migration flows.</t>
-  </si>
-  <si>
-    <t>Population Component of Medium (SSP2): This is the middle of the road scenario with Double migration flows.</t>
-  </si>
-  <si>
     <t>kccode</t>
   </si>
   <si>
@@ -308,6 +302,12 @@
   </si>
   <si>
     <t>Conventional Development (SSP5)</t>
+  </si>
+  <si>
+    <t>Population Component of Medium (SSP2): Middle of the road scenario with zero migration flows.</t>
+  </si>
+  <si>
+    <t>Population Component of Medium (SSP2): Middle of the road scenario with double migration flows.</t>
   </si>
 </sst>
 </file>
@@ -1142,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1166,13 +1166,13 @@
         <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1249,19 +1249,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E5">
         <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="G5" t="s">
         <v>68</v>
@@ -1272,19 +1272,19 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E6">
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="G6" t="s">
         <v>69</v>
@@ -1295,19 +1295,19 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C7">
         <v>7</v>
       </c>
       <c r="D7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
         <v>90</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1315,19 +1315,19 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C8">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E8">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -2125,7 +2125,7 @@
         <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -2139,7 +2139,7 @@
         <v>2</v>
       </c>
       <c r="G66" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -2187,7 +2187,7 @@
         <v>45</v>
       </c>
       <c r="G69" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -2204,7 +2204,7 @@
         <v>47</v>
       </c>
       <c r="G70" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -2221,7 +2221,7 @@
         <v>49</v>
       </c>
       <c r="G71" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -2238,7 +2238,7 @@
         <v>51</v>
       </c>
       <c r="G72" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
@@ -2252,10 +2252,10 @@
         <v>6</v>
       </c>
       <c r="F73" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G73" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -2272,7 +2272,7 @@
         <v>70</v>
       </c>
       <c r="G74" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>